<commit_message>
Clear particles at the start of optimization load.  This makes for less confusion since otherwise, the old particles will show while images are loaded before the optimizer starts.
</commit_message>
<xml_diff>
--- a/Examples/Studio/FeatureMap/feature_map_example.xlsx
+++ b/Examples/Studio/FeatureMap/feature_map_example.xlsx
@@ -13,18 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="groom" sheetId="10" r:id="rId2"/>
-    <sheet name="optimize" sheetId="11" r:id="rId3"/>
-    <sheet name="analysis" sheetId="12" r:id="rId4"/>
-    <sheet name="studio" sheetId="13" r:id="rId5"/>
-    <sheet name="project" sheetId="14" r:id="rId6"/>
+    <sheet name="groom" sheetId="15" r:id="rId2"/>
+    <sheet name="optimize" sheetId="16" r:id="rId3"/>
+    <sheet name="analysis" sheetId="17" r:id="rId4"/>
+    <sheet name="studio" sheetId="18" r:id="rId5"/>
+    <sheet name="project" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
   <si>
     <t>key</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Reconstructed</t>
+  </si>
+  <si>
+    <t>optimize</t>
+  </si>
+  <si>
+    <t>Groomed</t>
   </si>
 </sst>
 </file>
@@ -772,7 +778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -869,7 +875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -998,7 +1004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,7 +1045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1081,7 +1087,7 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1089,7 +1095,7 @@
         <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1097,14 +1103,14 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Adjust studio example params
</commit_message>
<xml_diff>
--- a/Examples/Studio/FeatureMap/feature_map_example.xlsx
+++ b/Examples/Studio/FeatureMap/feature_map_example.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/FeatureMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DAAE42-D71E-0942-80A9-758C3BAD7064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="460" windowWidth="15360" windowHeight="18740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="460" windowWidth="15360" windowHeight="18740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="groom" sheetId="2" r:id="rId2"/>
-    <sheet name="optimize" sheetId="3" r:id="rId3"/>
-    <sheet name="analysis" sheetId="4" r:id="rId4"/>
-    <sheet name="studio" sheetId="5" r:id="rId5"/>
-    <sheet name="project" sheetId="6" r:id="rId6"/>
+    <sheet name="groom" sheetId="14" r:id="rId2"/>
+    <sheet name="optimize" sheetId="15" r:id="rId3"/>
+    <sheet name="analysis" sheetId="16" r:id="rId4"/>
+    <sheet name="studio" sheetId="17" r:id="rId5"/>
+    <sheet name="project" sheetId="18" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>key</t>
   </si>
@@ -219,16 +218,7 @@
     <t>tool_state</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>view_state</t>
-  </si>
-  <si>
-    <t>Original</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>&lt;!DOCTYPE HTML PUBLIC "-//W3C//DTD HTML 4.0//EN" "http://www.w3.org/TR/REC-html40/strict.dtd"&gt;
@@ -242,11 +232,35 @@
 &lt;p style=" margin-top:12px; margin-bottom:12px; margin-left:0px; margin-right:0px; -qt-block-indent:0; text-indent:0px;"&gt;This example also demonstrates &lt;span style=" font-weight:600; font-style:italic;"&gt;group&lt;/span&gt; functionality.  Two of the shapes are associated with ‘left’ and the other two are in the ‘right’ group.  We can display the average feature map pattern on these two groups and also anywhere in-between. &lt;/p&gt;
 &lt;p style=" margin-top:12px; margin-bottom:12px; margin-left:0px; margin-right:0px; -qt-block-indent:0; text-indent:0px;"&gt;   &lt;/p&gt;&lt;/body&gt;&lt;/html&gt;</t>
   </si>
+  <si>
+    <t>0.050000</t>
+  </si>
+  <si>
+    <t>100.000000</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>analysis</t>
+  </si>
+  <si>
+    <t>Reconstructed</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -276,11 +290,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,9 +301,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -560,7 +568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -616,7 +624,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -632,17 +640,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -650,7 +653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -658,7 +661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -666,7 +669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -674,7 +677,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -682,7 +685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -690,7 +693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -698,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -706,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -714,7 +717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -722,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -731,21 +734,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,23 +750,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -777,15 +774,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -793,15 +790,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -809,15 +806,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -825,7 +822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -833,7 +830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -841,7 +838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -849,36 +846,32 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -894,7 +887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -902,7 +895,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -911,21 +904,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -941,7 +928,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -949,52 +936,48 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>63</v>
       </c>
       <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
       <c r="B6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1011,6 +994,5 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change Inference -> Testing.
</commit_message>
<xml_diff>
--- a/Examples/Studio/FeatureMap/feature_map_example.xlsx
+++ b/Examples/Studio/FeatureMap/feature_map_example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/FeatureMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4885A813-9416-BB42-B612-B0F4D881F438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="460" windowWidth="15360" windowHeight="18740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -18,13 +19,14 @@
     <sheet name="analysis" sheetId="16" r:id="rId4"/>
     <sheet name="studio" sheetId="17" r:id="rId5"/>
     <sheet name="project" sheetId="18" r:id="rId6"/>
+    <sheet name="deepssm" sheetId="19" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="127">
   <si>
     <t>key</t>
   </si>
@@ -159,9 +161,6 @@
   </si>
   <si>
     <t>version</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>segmentation_ellipsoid</t>
@@ -242,25 +241,187 @@
     <t>1000</t>
   </si>
   <si>
-    <t>analysis</t>
-  </si>
-  <si>
     <t>Reconstructed</t>
   </si>
   <si>
     <t>data</t>
   </si>
   <si>
-    <t>Original</t>
-  </si>
-  <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>value_ellipsoid</t>
+  </si>
+  <si>
+    <t>alignment_enabled</t>
+  </si>
+  <si>
+    <t>alignment_method</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>groom_output_prefix</t>
+  </si>
+  <si>
+    <t>groomed</t>
+  </si>
+  <si>
+    <t>mesh_smooth</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_method</t>
+  </si>
+  <si>
+    <t>Laplacian</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
+  </si>
+  <si>
+    <t>groomed_ellipsoid</t>
+  </si>
+  <si>
+    <t>alignment_ellipsoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -39.999849 -49.999811 -49.999811</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -42.499850 -50.000000 -50.000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -57.499850 -50.000000 -50.000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -59.999700 -49.999873 -49.999873</t>
+  </si>
+  <si>
+    <t>geodesic_cache_multiplier</t>
+  </si>
+  <si>
+    <t>narrow_band</t>
+  </si>
+  <si>
+    <t>4.000000</t>
+  </si>
+  <si>
+    <t>optimize_output_prefix</t>
+  </si>
+  <si>
+    <t>&lt;project&gt;_particles</t>
+  </si>
+  <si>
+    <t>use_geodesic_distance</t>
+  </si>
+  <si>
+    <t>local_particles_ellipsoid</t>
+  </si>
+  <si>
+    <t>world_particles_ellipsoid</t>
+  </si>
+  <si>
+    <t>aug_num_dims</t>
+  </si>
+  <si>
+    <t>aug_num_samples</t>
+  </si>
+  <si>
+    <t>aug_percent_variability</t>
+  </si>
+  <si>
+    <t>0.950000</t>
+  </si>
+  <si>
+    <t>aug_sampler_type</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
+  </si>
+  <si>
+    <t>train_decay_learning_rate</t>
+  </si>
+  <si>
+    <t>train_epochs</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>train_fine_tuning</t>
+  </si>
+  <si>
+    <t>train_learning_rate</t>
+  </si>
+  <si>
+    <t>0.001000</t>
+  </si>
+  <si>
+    <t>10/ellipsoid_1_DT.nrrd</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_1_DT_local.particles</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_1_DT_world.particles</t>
+  </si>
+  <si>
+    <t>10/ellipsoid_2_DT.nrrd</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_2_DT_local.particles</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_2_DT_world.particles</t>
+  </si>
+  <si>
+    <t>10/ellipsoid_3_DT.nrrd</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_3_DT_local.particles</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_3_DT_world.particles</t>
+  </si>
+  <si>
+    <t>10/ellipsoid_4_DT.nrrd</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_4_DT_local.particles</t>
+  </si>
+  <si>
+    <t>feature_map_example_particles/ellipsoid_4_DT_world.particles</t>
+  </si>
+  <si>
+    <t>group_hypertension</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>group_diabetes</t>
+  </si>
+  <si>
+    <t>group_stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -301,6 +462,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -568,71 +732,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
-        <v>58</v>
-      </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -640,109 +912,221 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -758,120 +1142,156 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -879,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -887,7 +1307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -895,7 +1315,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -904,15 +1324,19 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B7"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -920,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -928,56 +1352,60 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
       <c r="B6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -985,14 +1413,100 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update feature map example to have 6 shapes and more obvious L/R features.
</commit_message>
<xml_diff>
--- a/Examples/Studio/FeatureMap/feature_map_example.xlsx
+++ b/Examples/Studio/FeatureMap/feature_map_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/FeatureMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4885A813-9416-BB42-B612-B0F4D881F438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DC5567-927A-F24A-BAF2-3F8DF51B532F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
   <si>
     <t>key</t>
   </si>
@@ -175,33 +175,21 @@
     <t>ellipsoid_1.nrrd</t>
   </si>
   <si>
-    <t>feature_1.nrrd</t>
-  </si>
-  <si>
     <t>left</t>
   </si>
   <si>
     <t>ellipsoid_2.nrrd</t>
   </si>
   <si>
-    <t>feature_2.nrrd</t>
-  </si>
-  <si>
     <t>ellipsoid_3.nrrd</t>
   </si>
   <si>
-    <t>feature_3.nrrd</t>
-  </si>
-  <si>
     <t>right</t>
   </si>
   <si>
     <t>ellipsoid_4.nrrd</t>
   </si>
   <si>
-    <t>feature_4.nrrd</t>
-  </si>
-  <si>
     <t>500</t>
   </si>
   <si>
@@ -209,9 +197,6 @@
   </si>
   <si>
     <t>feature_map</t>
-  </si>
-  <si>
-    <t>sample</t>
   </si>
   <si>
     <t>tool_state</t>
@@ -241,181 +226,157 @@
     <t>1000</t>
   </si>
   <si>
-    <t>Reconstructed</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>value_ellipsoid</t>
+  </si>
+  <si>
+    <t>alignment_enabled</t>
+  </si>
+  <si>
+    <t>alignment_method</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>groom_output_prefix</t>
+  </si>
+  <si>
+    <t>groomed</t>
+  </si>
+  <si>
+    <t>mesh_smooth</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_method</t>
+  </si>
+  <si>
+    <t>Laplacian</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
+  </si>
+  <si>
+    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
+  </si>
+  <si>
+    <t>geodesic_cache_multiplier</t>
+  </si>
+  <si>
+    <t>narrow_band</t>
+  </si>
+  <si>
+    <t>4.000000</t>
+  </si>
+  <si>
+    <t>optimize_output_prefix</t>
+  </si>
+  <si>
+    <t>&lt;project&gt;_particles</t>
+  </si>
+  <si>
+    <t>use_geodesic_distance</t>
+  </si>
+  <si>
+    <t>aug_num_dims</t>
+  </si>
+  <si>
+    <t>aug_num_samples</t>
+  </si>
+  <si>
+    <t>aug_percent_variability</t>
+  </si>
+  <si>
+    <t>0.950000</t>
+  </si>
+  <si>
+    <t>aug_sampler_type</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
+  </si>
+  <si>
+    <t>train_decay_learning_rate</t>
+  </si>
+  <si>
+    <t>train_epochs</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>train_fine_tuning</t>
+  </si>
+  <si>
+    <t>train_learning_rate</t>
+  </si>
+  <si>
+    <t>0.001000</t>
+  </si>
+  <si>
+    <t>ellipsoid_5.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_6.nrrd</t>
+  </si>
+  <si>
+    <t>testing_split</t>
+  </si>
+  <si>
+    <t>20.000000</t>
+  </si>
+  <si>
+    <t>train_batch_size</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>train_fine_tuning_epochs</t>
+  </si>
+  <si>
+    <t>train_fine_tuning_learning_rate</t>
+  </si>
+  <si>
+    <t>validation_split</t>
+  </si>
+  <si>
+    <t>feature_auto_scale</t>
+  </si>
+  <si>
+    <t>feature_range_max</t>
+  </si>
+  <si>
+    <t>feature_range_min</t>
+  </si>
+  <si>
+    <t>feature_uniform_scale</t>
+  </si>
+  <si>
+    <t>left.nrrd</t>
+  </si>
+  <si>
+    <t>right.nrrd</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>0.000000</t>
   </si>
   <si>
     <t>data</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>value_ellipsoid</t>
-  </si>
-  <si>
-    <t>alignment_enabled</t>
-  </si>
-  <si>
-    <t>alignment_method</t>
-  </si>
-  <si>
-    <t>Center</t>
-  </si>
-  <si>
-    <t>groom_output_prefix</t>
-  </si>
-  <si>
-    <t>groomed</t>
-  </si>
-  <si>
-    <t>mesh_smooth</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_method</t>
-  </si>
-  <si>
-    <t>Laplacian</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_laplacian_iterations</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_laplacian_relaxation</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_windowed_sinc_iterations</t>
-  </si>
-  <si>
-    <t>mesh_smoothing_vtk_windowed_sinc_passband</t>
-  </si>
-  <si>
-    <t>groomed_ellipsoid</t>
-  </si>
-  <si>
-    <t>alignment_ellipsoid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -39.999849 -49.999811 -49.999811</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -42.499850 -50.000000 -50.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -57.499850 -50.000000 -50.000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -59.999700 -49.999873 -49.999873</t>
-  </si>
-  <si>
-    <t>geodesic_cache_multiplier</t>
-  </si>
-  <si>
-    <t>narrow_band</t>
-  </si>
-  <si>
-    <t>4.000000</t>
-  </si>
-  <si>
-    <t>optimize_output_prefix</t>
-  </si>
-  <si>
-    <t>&lt;project&gt;_particles</t>
-  </si>
-  <si>
-    <t>use_geodesic_distance</t>
-  </si>
-  <si>
-    <t>local_particles_ellipsoid</t>
-  </si>
-  <si>
-    <t>world_particles_ellipsoid</t>
-  </si>
-  <si>
-    <t>aug_num_dims</t>
-  </si>
-  <si>
-    <t>aug_num_samples</t>
-  </si>
-  <si>
-    <t>aug_percent_variability</t>
-  </si>
-  <si>
-    <t>0.950000</t>
-  </si>
-  <si>
-    <t>aug_sampler_type</t>
-  </si>
-  <si>
-    <t>Gaussian</t>
-  </si>
-  <si>
-    <t>train_decay_learning_rate</t>
-  </si>
-  <si>
-    <t>train_epochs</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>train_fine_tuning</t>
-  </si>
-  <si>
-    <t>train_learning_rate</t>
-  </si>
-  <si>
-    <t>0.001000</t>
-  </si>
-  <si>
-    <t>10/ellipsoid_1_DT.nrrd</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_1_DT_local.particles</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_1_DT_world.particles</t>
-  </si>
-  <si>
-    <t>10/ellipsoid_2_DT.nrrd</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_2_DT_local.particles</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_2_DT_world.particles</t>
-  </si>
-  <si>
-    <t>10/ellipsoid_3_DT.nrrd</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_3_DT_local.particles</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_3_DT_world.particles</t>
-  </si>
-  <si>
-    <t>10/ellipsoid_4_DT.nrrd</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_4_DT_local.particles</t>
-  </si>
-  <si>
-    <t>feature_map_example_particles/ellipsoid_4_DT_world.particles</t>
-  </si>
-  <si>
-    <t>group_hypertension</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>group_diabetes</t>
-  </si>
-  <si>
-    <t>group_stage</t>
   </si>
 </sst>
 </file>
@@ -733,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,10 +705,9 @@
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -757,154 +717,71 @@
       <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" t="s">
-        <v>124</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -928,12 +805,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -944,13 +821,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1032,13 +909,13 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1051,7 +928,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1059,15 +936,15 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1075,7 +952,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
@@ -1083,7 +960,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1091,10 +968,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1144,7 +1021,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -1155,7 +1032,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1163,7 +1040,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1184,10 +1061,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1203,7 +1080,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1211,15 +1088,15 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,12 +1136,12 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
@@ -1330,11 +1207,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1354,42 +1236,74 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
+      <c r="B11" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1418,7 +1332,7 @@
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1428,7 +1342,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1444,7 +1358,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -1452,7 +1366,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1460,39 +1374,39 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1500,10 +1414,50 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add interface and infrastrucutre for shape scalar correlation.
</commit_message>
<xml_diff>
--- a/Examples/Studio/FeatureMap/feature_map_example.xlsx
+++ b/Examples/Studio/FeatureMap/feature_map_example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="174">
   <si>
     <t>name</t>
   </si>
@@ -384,6 +384,15 @@
   </si>
   <si>
     <t>use_landmarks</t>
+  </si>
+  <si>
+    <t>use_geodesics_to_landmarks</t>
+  </si>
+  <si>
+    <t>geodesics_to_landmarks_weight</t>
+  </si>
+  <si>
+    <t>use_disentangled_ssm</t>
   </si>
   <si>
     <t>analysis_mode</t>
@@ -428,13 +437,13 @@
     <t>tool_state</t>
   </si>
   <si>
-    <t>optimize</t>
+    <t>analysis</t>
   </si>
   <si>
     <t>view_state</t>
   </si>
   <si>
-    <t>Groomed</t>
+    <t>Reconstructed</t>
   </si>
   <si>
     <t>zoom_state</t>
@@ -1437,7 +1446,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1605,6 +1614,30 @@
         <v>120</v>
       </c>
       <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1627,15 +1660,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -1643,15 +1676,15 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
         <v>116</v>
@@ -1659,7 +1692,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
@@ -1667,7 +1700,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -1675,34 +1708,34 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +1757,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
         <v>46</v>
@@ -1749,50 +1782,50 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1814,55 +1847,55 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
@@ -1870,15 +1903,15 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
@@ -1886,7 +1919,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
@@ -1894,26 +1927,26 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1927,19 +1960,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>